<commit_message>
replace excel2json templates by new version
</commit_message>
<xml_diff>
--- a/data_model_files/import (The template ontology for data import)/properties.xlsx
+++ b/data_model_files/import (The template ontology for data import)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/knora/dsplib/import_scripts/data_model_files/import (The template ontology for data import)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/src/dsp_tools/import_scripts/data_model_files/import (The template ontology for data import)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B12987-5265-A941-8340-567014F3F422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC80602-9603-2444-8890-16719D06F687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="29580" windowHeight="17820" xr2:uid="{352B9572-BD89-B646-9758-957DE76BD52A}"/>
   </bookViews>
@@ -32,6 +32,347 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Johannes Nussbaum</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2AA75EB4-F9D8-7B48-90FD-E686FA8C2D30}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Unique identifier for the property</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{56A4B07A-41CF-5F4F-8194-7BD663F9CA61}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">one language mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Label of the property that will be displayed in DSP-APP. Should be rather short. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{0CCD675D-6735-814E-B506-EC343F6BD11B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">optional
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Description of the property. Can be longer than the label.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{BC9ECCAC-D59A-7947-8387-8573F52F941E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The type of this property, i.e. the base property/ies that this property is derived from. Must be one of the values listed in the documentation.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If more than one: separated by commas.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{B063DCF9-2B76-5D4D-963C-62F8FEBDC451}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Target value of this property. Must be one of the values listed in the documentation. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">If the property is derived from hasValue, the type of the property must be further specified by the object it takes, e.g. TextValue, ListValue, or IntValue. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If the property is derived from hasLinkTo, the object specifies the resource class that this property refers to.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{9786AB60-F20E-304C-813F-7E7526474E32}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mandatory
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The graphic component, defines how this property should be displayed. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Depends on the value of "object". Read the documentation of the respective "object" to learn which "gui_element" can be used.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{925FD375-684C-E845-98C6-24590B304DAF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">only mandatory for lists
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Some "gui_elements" need further specification. Read the documentation of the respective "object" to learn if your "gui_element" needs a "gui_attributes".
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="+mn-lt"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Form: "attr: value, attr: value". </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
@@ -44,21 +385,6 @@
     <t>object</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>rm</t>
-  </si>
-  <si>
     <t>comment_en</t>
   </si>
   <si>
@@ -216,13 +542,28 @@
   </si>
   <si>
     <t>Checkbox</t>
+  </si>
+  <si>
+    <t>label_en</t>
+  </si>
+  <si>
+    <t>label_de</t>
+  </si>
+  <si>
+    <t>label_fr</t>
+  </si>
+  <si>
+    <t>label_it</t>
+  </si>
+  <si>
+    <t>label_rm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,6 +578,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="+mn-lt"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -256,14 +620,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -575,285 +942,296 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB295ED-2B92-7F4D-AD0D-5345A9E34A8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB295ED-2B92-7F4D-AD0D-5345A9E34A8B}">
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.83203125" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N3" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="N8" t="s">
         <v>35</v>
       </c>
-      <c r="N5" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N6" t="s">
-        <v>19</v>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="N7" t="s">
-        <v>16</v>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="N8" t="s">
-        <v>40</v>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" t="s">
-        <v>19</v>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="N10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" t="s">
         <v>53</v>
       </c>
-      <c r="N11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="N13" t="s">
         <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-      <c r="N12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N13" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G1" r:id="rId1" location="property-comments" xr:uid="{EA536852-5B63-BE4A-9F2F-32B131302D7B}"/>
+    <hyperlink ref="L1" r:id="rId2" location="property-super" xr:uid="{F70581CB-359A-8246-888D-185591710323}"/>
+    <hyperlink ref="M1" r:id="rId3" location="property-object-gui_element-gui_attributes" xr:uid="{A98E3DD3-C597-2A48-B4BA-1E5B782A1E93}"/>
+    <hyperlink ref="N1" r:id="rId4" location="property-object-gui_element-gui_attributes" xr:uid="{E691A69D-28FB-884F-9359-76DDE591C7FD}"/>
+    <hyperlink ref="O1" r:id="rId5" location="property-object-gui_element-gui_attributes" xr:uid="{6822D067-F25B-3143-88B0-BF685141B9D2}"/>
+    <hyperlink ref="A1" r:id="rId6" location="property-name" xr:uid="{BE262A33-3433-B34D-A7AC-41254080C6C2}"/>
+    <hyperlink ref="B1" r:id="rId7" location="property-labels" xr:uid="{5E203058-8C63-4042-A957-9564EF9ABC0C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>